<commit_message>
tried to add validity checker for connection investment type.
</commit_message>
<xml_diff>
--- a/example_data/connections/connections-input.xlsx
+++ b/example_data/connections/connections-input.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,6 +592,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L1003" type="list">
+      <formula1>"connection_investment_variable_type_continuous,connection_investment_variable_type_integer"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>